<commit_message>
feat: all test cases added together
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\juani\eclipse-workspace\SeleniumMavenFramewoork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET ACADEMY PROJECT\SeleniumMavenFramewoork\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9C45D2-9369-4D84-A4A5-704D7E1C86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="43650" yWindow="1635" windowWidth="18390" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Jm1234</t>
   </si>
@@ -41,34 +42,70 @@
     <t>email</t>
   </si>
   <si>
-    <t>jvl1275s001</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
-    <t>chusername</t>
-  </si>
-  <si>
-    <t>jul1o</t>
-  </si>
-  <si>
-    <t>A1234*l</t>
-  </si>
-  <si>
-    <t>chpassword</t>
-  </si>
-  <si>
-    <t>pusername</t>
-  </si>
-  <si>
-    <t>ppassword</t>
+    <t>item</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>gael</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>gonzalez</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>n1235454</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>mexico</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>ensenada</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>cercas</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>baja</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>c22880</t>
+  </si>
+  <si>
+    <t>julzzz1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,8 +135,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,27 +422,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -407,7 +450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -415,7 +458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -423,36 +466,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: payment order validation and comments added
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SDET ACADEMY PROJECT\SeleniumMavenFramewoork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9C45D2-9369-4D84-A4A5-704D7E1C86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E84317F-A511-4719-BACD-0347B6B3F39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43650" yWindow="1635" windowWidth="18390" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
     <t>c22880</t>
   </si>
   <si>
-    <t>julzzz1</t>
+    <t>jul3084dz1</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>